<commit_message>
fixed data path hard code
</commit_message>
<xml_diff>
--- a/finance/richtato/static/data/master_creditcard_data.xlsx
+++ b/finance/richtato/static/data/master_creditcard_data.xlsx
@@ -485,20 +485,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI</t>
+          <t>AplPay A2 PCI PARKINIRVINE              CA</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>73.59999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Parking</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -517,20 +517,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AplPay A2 PCI PARKINIRVINE              CA</t>
+          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2.4</v>
+        <v>73.59999999999999</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Parking</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>189.53</v>
+        <v>-11.99</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-11.99</v>
+        <v>189.53</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23.01</v>
+        <v>0.78</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -805,20 +805,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Tesla Inc Supercharger 877-7983752 CA</t>
+          <t>BOYNE MTN F&amp;B -DIN BOYNE FALLS MI</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.78</v>
+        <v>139</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -837,20 +837,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BOYNE MTN F&amp;B -DIN BOYNE FALLS MI</t>
+          <t>Tesla Inc Supercharger 877-7983752 CA</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>139</v>
+        <v>17.2</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>17.2</v>
+        <v>23.01</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -933,20 +933,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Tesla Inc Supercharger 877-7983752 CA</t>
+          <t>AplPay A2 PCI PARKINIRVINE              CA</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>29.64</v>
+        <v>2.4</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Parking</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -965,20 +965,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>AplPay A2 PCI PARKINIRVINE              CA</t>
+          <t>STARBUCKS 800-782-7282 800-782-7282 WA null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>2.4</v>
+        <v>25</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Parking</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1029,20 +1029,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>STARBUCKS 800-782-7282 800-782-7282 WA null XXXXXXXXXXXX9868</t>
+          <t>Tesla Inc Supercharger 877-7983752 CA</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>25</v>
+        <v>29.64</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1413,20 +1413,20 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Tesla Inc Supercharger 877-7983752 CA</t>
+          <t>AplPay MEIJER STORE HOLLAND             MI</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>11.22</v>
+        <v>2.32</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1445,20 +1445,20 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>AplPay MEIJER STORE HOLLAND             MI</t>
+          <t>TST* MIZU SUSHI Holland MI</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.32</v>
+        <v>70</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1477,20 +1477,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TST* MIZU SUSHI Holland MI</t>
+          <t>Tesla Inc Supercharger 877-7983752 CA</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>70</v>
+        <v>11.22</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1605,20 +1605,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>CHIPOTLE 1158 ANN ARBOR MI null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>151.83</v>
+        <v>12.67</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1669,20 +1669,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>CHIPOTLE 1158 ANN ARBOR MI null XXXXXXXXXXXX9868</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>12.67</v>
+        <v>151.83</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1701,20 +1701,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>AMEX RIDESHARE CREDIT</t>
+          <t>Subway 25044 7344857827 MI null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1770,15 +1770,15 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>AMAZON MARKEPLACE NA  PA</t>
+          <t>AMEX RIDESHARE CREDIT</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>31.4</v>
+        <v>-10</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -1797,20 +1797,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Subway 25044 7344857827 MI null XXXXXXXXXXXX9868</t>
+          <t>AMAZON MARKEPLACE NA  PA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>10</v>
+        <v>31.4</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -1893,20 +1893,20 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>INTUIT *TURBOTAX    800-446-8848        CA</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>40</v>
+        <v>-35.99</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1957,20 +1957,20 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>INTUIT *TURBOTAX    800-446-8848        CA</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>265.75</v>
+        <v>40</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -1998,7 +1998,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>-35.99</v>
+        <v>265.75</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -2026,15 +2026,15 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>USCUSTOMS TRUSTEDTRAINDIANAPOLIS        IN</t>
+          <t>INTUIT *TURBOTAX    800-446-8848        CA</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2058,15 +2058,15 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>INTUIT *TURBOTAX    800-446-8848        CA</t>
+          <t>ANN ARBOR COFFEE ROAAnn Arbor           MI</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>42.4</v>
+        <v>5.57</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -2094,7 +2094,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>40</v>
+        <v>42.4</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -2122,15 +2122,15 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ANN ARBOR COFFEE ROAAnn Arbor           MI</t>
+          <t>USCUSTOMS TRUSTEDTRAINDIANAPOLIS        IN</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>5.57</v>
+        <v>100</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -2186,15 +2186,15 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SLURPING TURTLE - ANANN ARBOR           MI</t>
+          <t>A2 PCI PARKING 82 RAIRVINE              CA</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>68.3</v>
+        <v>3.6</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Parking</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2218,15 +2218,15 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>A2 PCI PARKING 82 RAIRVINE              CA</t>
+          <t>SLURPING TURTLE - ANANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>3.6</v>
+        <v>68.3</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Parking</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -2250,15 +2250,15 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MACHEKO GRILLE 14500YPSILANTI           MI</t>
+          <t>AV ANN ARBOR        Ann Arbor           MI</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Fun</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2314,15 +2314,15 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>AV ANN ARBOR        Ann Arbor           MI</t>
+          <t>MACHEKO GRILLE 14500YPSILANTI           MI</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Fun</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F59" t="n">
@@ -2730,15 +2730,15 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>AMAZON.COM          AMZN.COM/BILL       WA</t>
+          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>8.460000000000001</v>
+        <v>11.13</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F72" t="n">
@@ -2794,15 +2794,15 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
+          <t>AMAZON.COM          AMZN.COM/BILL       WA</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>11.13</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F74" t="n">
@@ -2826,15 +2826,15 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>SP DIRTY LABS INC.  SCOTTSDALE          AZ</t>
+          <t>AplPay TESLA NEVADA Sparks              NV</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>38.14</v>
+        <v>10.68</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -2858,15 +2858,15 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>AplPay TESLA NEVADA Sparks              NV</t>
+          <t>SP DIRTY LABS INC.  SCOTTSDALE          AZ</t>
         </is>
       </c>
       <c r="D76" t="n">
-        <v>10.68</v>
+        <v>38.14</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -2922,11 +2922,11 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>AplPay IJJI NOODLE Hsparks              NV</t>
+          <t>AplPay HAND CRAFT COSparks              NV</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>12.26</v>
+        <v>3.65</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2954,11 +2954,11 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>AplPay HAND CRAFT COSparks              NV</t>
+          <t>AplPay IJJI NOODLE Hsparks              NV</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>8.98</v>
+        <v>12.26</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2990,7 +2990,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>3.65</v>
+        <v>8.98</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -3050,15 +3050,15 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>AplPay IJJI NOODLE Hsparks              NV</t>
+          <t>MEMBERSHIP FEE</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>12.26</v>
+        <v>350</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="F82" t="n">
@@ -3082,11 +3082,11 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>AplPay ROUNDABOUT GRSparks              NV</t>
+          <t>AplPay IJJI NOODLE Hsparks              NV</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>12.16</v>
+        <v>12.26</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -3146,15 +3146,15 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>MEMBERSHIP FEE</t>
+          <t>AplPay ROUNDABOUT GRSparks              NV</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>350</v>
+        <v>12.16</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -3242,15 +3242,15 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>HANCOOK. 0001       OAKLAND             CA</t>
+          <t>AplPay WHOLE FOODS MFREMONT             CA</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>285.37</v>
+        <v>18.73</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -3274,11 +3274,11 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>AplPay YOGURT PARK IBERKELEY            CA</t>
+          <t>HANCOOK. 0001       OAKLAND             CA</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>4.5</v>
+        <v>285.37</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -3306,15 +3306,15 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>AplPay WHOLE FOODS MFREMONT             CA</t>
+          <t>THE HOME DEPOT      FREMONT             CA</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>18.73</v>
+        <v>6.92</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -3466,15 +3466,15 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>AplPay SPOTHERO 844-CHICAGO             IL</t>
+          <t>AplPay LYFT         855-280-0278        CA</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>10.75</v>
+        <v>30.91</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Parking</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F95" t="n">
@@ -3498,15 +3498,15 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>AMEX RIDESHARE CREDIT</t>
+          <t>AplPay SPOTHERO 844-CHICAGO             IL</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>-10</v>
+        <v>10.75</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Parking</t>
         </is>
       </c>
       <c r="F96" t="n">
@@ -3530,15 +3530,15 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>THE HOME DEPOT      FREMONT             CA</t>
+          <t>AplPay YOGURT PARK IBERKELEY            CA</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>6.92</v>
+        <v>4.5</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F97" t="n">
@@ -3557,20 +3557,20 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>SONOS INC.          SANTA BARBARA       CA</t>
+          <t>AMEX RIDESHARE CREDIT</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>187.41</v>
+        <v>-10</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F98" t="n">
@@ -3589,20 +3589,20 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>AplPay LYFT         855-280-0278        CA</t>
+          <t>SONOS INC.          SANTA BARBARA       CA</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>30.91</v>
+        <v>187.41</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -3630,7 +3630,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0.75</v>
+        <v>0.3</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -3658,15 +3658,15 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #0778 FREMONT CA</t>
+          <t>BERKELEY-PRKG IPS METER BERKELEY CA</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>99.7</v>
+        <v>0.75</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Parking</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -3690,15 +3690,15 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>BERKELEY-PRKG IPS METER BERKELEY CA</t>
+          <t>COSTCO WHSE #0778 FREMONT CA</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0.3</v>
+        <v>99.7</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Parking</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F102" t="n">
@@ -3722,11 +3722,11 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>AplPay IMPERIAL TEA San Francisco       CA</t>
+          <t>RANTEI JAPANESE CUISSANTA CLARA         CA</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>6.25</v>
+        <v>146.6</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3754,15 +3754,15 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>AplPay SAY YA PHOTO SAN FRANCISCO       CA</t>
+          <t>TST* YANK SING - SPESAN FRANCISCO       CA</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>5.53</v>
+        <v>123.72</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F104" t="n">
@@ -3786,15 +3786,15 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>AplPay SP MAISON VERVALLEJO             CA</t>
+          <t>AplPay SAY YA PHOTO SAN FRANCISCO       CA</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>16</v>
+        <v>5.53</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="F105" t="n">
@@ -3818,11 +3818,11 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>RANTEI JAPANESE CUISSANTA CLARA         CA</t>
+          <t>AplPay IMPERIAL TEA San Francisco       CA</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>146.6</v>
+        <v>6.25</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3850,11 +3850,11 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>TST* YANK SING - SPESAN FRANCISCO       CA</t>
+          <t>AplPay SP MAISON VERVALLEJO             CA</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>123.72</v>
+        <v>16</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3946,11 +3946,11 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>RAMEN NAGI VALLEY FASan Jose            CA</t>
+          <t>AplPay OLIVE GARDEN FREMONT             CA</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>43.04</v>
+        <v>58.51</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3978,11 +3978,11 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>AplPay OLIVE GARDEN FREMONT             CA</t>
+          <t>RAMEN NAGI VALLEY FASan Jose            CA</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>58.51</v>
+        <v>43.04</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -4042,11 +4042,11 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
+          <t>TST* HIGH FLYING FOOSAUSALITO           CA</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>11.4</v>
+        <v>6.03</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -4074,11 +4074,11 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>TST* HIGH FLYING FOOSAUSALITO           CA</t>
+          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>6.03</v>
+        <v>11.4</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -4101,20 +4101,20 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>AT&amp;T UVERSE PAYMENT 8002882020          TX</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>103.36</v>
+        <v>55.22</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="F115" t="n">
@@ -4133,20 +4133,20 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>UBER</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>38.95</v>
+        <v>103.36</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F116" t="n">
@@ -4170,15 +4170,15 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
+          <t>UBER</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>20.53</v>
+        <v>38.95</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F117" t="n">
@@ -4197,20 +4197,20 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>AT&amp;T UVERSE PAYMENT 8002882020          TX</t>
+          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>55.22</v>
+        <v>20.53</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F118" t="n">
@@ -4234,11 +4234,11 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>AplPay SWEETWATERS CAnn Arbor           MI</t>
+          <t>AplPay CHIPOTLE 1219ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>4.88</v>
+        <v>11.13</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -4266,11 +4266,11 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>AplPay CHIPOTLE 1219ANN ARBOR           MI</t>
+          <t>AplPay SWEETWATERS CAnn Arbor           MI</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>11.13</v>
+        <v>4.88</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -4330,15 +4330,15 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>TST* TOMUKUN KOREAN ANN ARBOR           MI</t>
+          <t>AMAZON MARKEPLACE NA PA</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>25</v>
+        <v>931.74</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F122" t="n">
@@ -4394,15 +4394,15 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>AMAZON MARKEPLACE NA PA</t>
+          <t>TST* TOMUKUN KOREAN ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>931.74</v>
+        <v>25</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F124" t="n">
@@ -4549,20 +4549,20 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>ZIPPY AUTO WASH ANN ARBOR MI</t>
+          <t>DELTA AIR LINES</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>35.99</v>
+        <v>38.99</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Car Maintenance</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F129" t="n">
@@ -4586,15 +4586,15 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>EV CONNECT, INC. 866-816-7584 CA</t>
+          <t>ZIPPY AUTO WASH ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>3.05</v>
+        <v>35.99</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Car Maintenance</t>
         </is>
       </c>
       <c r="F130" t="n">
@@ -4613,20 +4613,20 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>DELTA AIR LINES</t>
+          <t>EV CONNECT, INC. 866-816-7584 CA</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>38.99</v>
+        <v>3.05</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F131" t="n">
@@ -4778,15 +4778,15 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Airport duty free   INCHEON</t>
+          <t>UBER</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>33.56</v>
+        <v>28.97</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F136" t="n">
@@ -4810,15 +4810,15 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>UBER</t>
+          <t>Airport duty free   INCHEON</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>28.97</v>
+        <v>33.56</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F137" t="n">
@@ -4906,11 +4906,11 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>AplPay CHIPOTLE 1219ANN ARBOR           MI</t>
+          <t>AplPay STARBUCKS    800-782-7282        WA</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>8.59</v>
+        <v>25</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -4938,11 +4938,11 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>AplPay STARBUCKS    800-782-7282        WA</t>
+          <t>AplPay CHIPOTLE 1219ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>25</v>
+        <v>8.59</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -4970,15 +4970,15 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>AplPay TARGET       ANN ARBOR           MI</t>
+          <t>AplPay GINGER DELI  Ann Arbor           MI</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>16.47</v>
+        <v>1.06</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F142" t="n">
@@ -5002,15 +5002,15 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>THE SEOUL 1450000027ANN ARBOR           MI</t>
+          <t>A2 PCI PARKING 87 RAIRVINE              CA</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>73.16</v>
+        <v>2.4</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Parking</t>
         </is>
       </c>
       <c r="F143" t="n">
@@ -5034,15 +5034,15 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>A2 PCI PARKING 87 RAIRVINE              CA</t>
+          <t>THE SEOUL 1450000027ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D144" t="n">
-        <v>2.4</v>
+        <v>73.16</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Parking</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F144" t="n">
@@ -5098,15 +5098,15 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>AplPay GINGER DELI  Ann Arbor           MI</t>
+          <t>AplPay TARGET       ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D146" t="n">
-        <v>1.06</v>
+        <v>16.47</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F146" t="n">
@@ -5194,15 +5194,15 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>AplPay TARGET       ANN ARBOR           MI</t>
+          <t>TST* TOMUKUN KOREAN ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>4.65</v>
+        <v>18.6</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F149" t="n">
@@ -5226,15 +5226,15 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>TST* TOMUKUN KOREAN ANN ARBOR           MI</t>
+          <t>AplPay TARGET       ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>18.6</v>
+        <v>4.65</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F150" t="n">
@@ -5418,15 +5418,15 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
+          <t>AMAZON MARKETPLACE NAMZN.COM/BILL       WA</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>18.75</v>
+        <v>-931.74</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F156" t="n">
@@ -5450,15 +5450,15 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>AMAZON.COM          AMZN.COM/BILL       WA</t>
+          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
         </is>
       </c>
       <c r="D157" t="n">
-        <v>200.34</v>
+        <v>18.75</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F157" t="n">
@@ -5482,11 +5482,11 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>AMAZON MARKETPLACE NAMZN.COM/BILL       WA</t>
+          <t>AMAZON.COM          AMZN.COM/BILL       WA</t>
         </is>
       </c>
       <c r="D158" t="n">
-        <v>-931.74</v>
+        <v>200.34</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -5578,11 +5578,11 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>AplPay WHOLE FOODS MANN ARBOR           MI</t>
+          <t>AplPay TRADER JOE S ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>5.99</v>
+        <v>7.98</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -5642,11 +5642,11 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>AplPay TRADER JOE S ANN ARBOR           MI</t>
+          <t>AplPay WHOLE FOODS MANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D163" t="n">
-        <v>7.98</v>
+        <v>5.99</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -5669,20 +5669,20 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>AT&amp;T UVERSE PAYMENT 8002882020          TX</t>
+          <t>AMAZON MARKEPLACE NA  PA</t>
         </is>
       </c>
       <c r="D164" t="n">
-        <v>55.22</v>
+        <v>44.09</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F164" t="n">
@@ -5706,15 +5706,15 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>USPS PO 2599760197 0YPSILANTI           MI</t>
+          <t>AT&amp;T UVERSE PAYMENT 8002882020          TX</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>10.8</v>
+        <v>55.22</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="F165" t="n">
@@ -5733,20 +5733,20 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>AMAZON MARKEPLACE NA  PA</t>
+          <t>USPS PO 2599760197 0YPSILANTI           MI</t>
         </is>
       </c>
       <c r="D166" t="n">
-        <v>44.09</v>
+        <v>10.8</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="F166" t="n">
@@ -5829,20 +5829,20 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>AplPay BUSCH'S VALU ANN ARBOR           MI</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>14.9</v>
+        <v>-21.19</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F169" t="n">
@@ -5893,20 +5893,20 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>AplPay BUSCH'S VALU ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>-21.19</v>
+        <v>14.9</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F171" t="n">
@@ -5925,20 +5925,20 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>ZIPPY AUTO WASH ANN ARBOR MI</t>
+          <t>APPLE.COM/BILL      INTERNET CHARGE     CA</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>35.99</v>
+        <v>10.99</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Car Maintenance</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="F172" t="n">
@@ -5957,20 +5957,20 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>APPLE.COM/BILL      INTERNET CHARGE     CA</t>
+          <t>ZIPPY AUTO WASH ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D173" t="n">
-        <v>10.99</v>
+        <v>35.99</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Car Maintenance</t>
         </is>
       </c>
       <c r="F173" t="n">
@@ -6085,20 +6085,20 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>AMAZON.COM          AMZN.COM/BILL       WA</t>
+          <t>AplPay WHOLEFDS CRB ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D177" t="n">
-        <v>3.99</v>
+        <v>11.59</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F177" t="n">
@@ -6117,20 +6117,20 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>AplPay WHOLEFDS CRB ANN ARBOR           MI</t>
+          <t>AMAZON.COM          AMZN.COM/BILL       WA</t>
         </is>
       </c>
       <c r="D178" t="n">
-        <v>11.59</v>
+        <v>3.99</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F178" t="n">
@@ -6149,20 +6149,20 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
         </is>
       </c>
       <c r="D179" t="n">
-        <v>14.99</v>
+        <v>2.86</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F179" t="n">
@@ -6181,20 +6181,20 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D180" t="n">
-        <v>2.86</v>
+        <v>14.99</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F180" t="n">
@@ -6469,16 +6469,16 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>AplPay TARGET       ANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D189" t="n">
-        <v>92.15000000000001</v>
+        <v>21.72</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -6501,20 +6501,20 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D190" t="n">
-        <v>18.11</v>
+        <v>92.15000000000001</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F190" t="n">
@@ -6538,15 +6538,15 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>AplPay TARGET       ANN ARBOR           MI</t>
+          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
         </is>
       </c>
       <c r="D191" t="n">
-        <v>21.72</v>
+        <v>18.11</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F191" t="n">
@@ -6629,20 +6629,20 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
+          <t>AMAZON MARKETPLACE NAMZN.COM/BILL       WA</t>
         </is>
       </c>
       <c r="D194" t="n">
-        <v>18.11</v>
+        <v>-44.09</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F194" t="n">
@@ -6661,20 +6661,20 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>AMAZON MARKETPLACE NAMZN.COM/BILL       WA</t>
+          <t>AplPay ROSEWAY SUB, TAYLOR              MI</t>
         </is>
       </c>
       <c r="D195" t="n">
-        <v>-44.09</v>
+        <v>18.11</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F195" t="n">
@@ -6693,20 +6693,20 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D196" t="n">
-        <v>37</v>
+        <v>94.76000000000001</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F196" t="n">
@@ -6725,20 +6725,20 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI</t>
         </is>
       </c>
       <c r="D197" t="n">
-        <v>94.76000000000001</v>
+        <v>37</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F197" t="n">
@@ -6789,20 +6789,20 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
+          <t>AplPay WHOLE FOODS MANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D199" t="n">
-        <v>12.67</v>
+        <v>11.98</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F199" t="n">
@@ -6826,15 +6826,15 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>AplPay K&amp;D BISTRO 00YPSILANTI           MI</t>
+          <t>AplPay 9651 GREAT CLANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D200" t="n">
-        <v>13.73</v>
+        <v>27</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="F200" t="n">
@@ -6853,20 +6853,20 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>AplPay WHOLE FOODS MANN ARBOR           MI</t>
+          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
         </is>
       </c>
       <c r="D201" t="n">
-        <v>11.98</v>
+        <v>12.67</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F201" t="n">
@@ -6890,15 +6890,15 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>AplPay 9651 GREAT CLANN ARBOR           MI</t>
+          <t>AplPay K&amp;D BISTRO 00YPSILANTI           MI</t>
         </is>
       </c>
       <c r="D202" t="n">
-        <v>27</v>
+        <v>13.73</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F202" t="n">
@@ -6917,16 +6917,16 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>AplPay STARBUCKS    800-782-7282        WA</t>
+          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D203" t="n">
-        <v>25</v>
+        <v>24.8</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -6949,16 +6949,16 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI null XXXXXXXXXXXX9868</t>
+          <t>AplPay STARBUCKS    800-782-7282        WA</t>
         </is>
       </c>
       <c r="D204" t="n">
-        <v>24.8</v>
+        <v>25</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -7013,20 +7013,20 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
+          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
         </is>
       </c>
       <c r="D206" t="n">
-        <v>106</v>
+        <v>12.67</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F206" t="n">
@@ -7045,20 +7045,20 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>AplPay CHIPOTLE ONLINEWPORT BEACH       CA</t>
+          <t>COSTCO WHSE #1106 ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D207" t="n">
-        <v>12.67</v>
+        <v>106</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F207" t="n">
@@ -7109,20 +7109,20 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #0144 SAN FRANCISCOCA</t>
+          <t>TST* CLEAN JUICE - CAS GRAND RAPIDS MI null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D209" t="n">
-        <v>200.86</v>
+        <v>11.61</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F209" t="n">
@@ -7141,20 +7141,20 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>APPLE.COM/BILL      INTERNET CHARGE     CA</t>
+          <t>TESLA SUPERCHARGER US 877-7983752 CA</t>
         </is>
       </c>
       <c r="D210" t="n">
-        <v>9.99</v>
+        <v>6.84</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F210" t="n">
@@ -7173,20 +7173,20 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>TESLA SUPERCHARGER US 877-7983752 CA</t>
+          <t>AplPay DICK'S SPORTICORAOPOLIS          PA</t>
         </is>
       </c>
       <c r="D211" t="n">
-        <v>18.72</v>
+        <v>84.79000000000001</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F211" t="n">
@@ -7205,20 +7205,20 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
+          <t>COSTCO WHSE #0144 SAN FRANCISCOCA</t>
         </is>
       </c>
       <c r="D212" t="n">
-        <v>10.06</v>
+        <v>200.86</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F212" t="n">
@@ -7237,20 +7237,20 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>AplPay DICK'S SPORTICORAOPOLIS          PA</t>
+          <t>TESLA SUPERCHARGER US 877-7983752 CA</t>
         </is>
       </c>
       <c r="D213" t="n">
-        <v>84.79000000000001</v>
+        <v>18.72</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F213" t="n">
@@ -7269,20 +7269,20 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>TESLA SUPERCHARGER US 877-7983752 CA</t>
+          <t>APPLE.COM/BILL      INTERNET CHARGE     CA</t>
         </is>
       </c>
       <c r="D214" t="n">
-        <v>6.84</v>
+        <v>9.99</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="F214" t="n">
@@ -7301,20 +7301,20 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>TST* CLEAN JUICE - CAS GRAND RAPIDS MI null XXXXXXXXXXXX9868</t>
+          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
         </is>
       </c>
       <c r="D215" t="n">
-        <v>11.61</v>
+        <v>10.06</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F215" t="n">
@@ -7365,20 +7365,20 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI</t>
+          <t>AplPay DICK'S SPORTICORAOPOLIS          PA</t>
         </is>
       </c>
       <c r="D217" t="n">
-        <v>25</v>
+        <v>-84.79000000000001</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F217" t="n">
@@ -7397,20 +7397,20 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>AplPay DICK'S SPORTICORAOPOLIS          PA</t>
+          <t>TST* TOMUKUN KOREAN BB Ann Arbor MI</t>
         </is>
       </c>
       <c r="D218" t="n">
-        <v>-84.79000000000001</v>
+        <v>25</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -7557,20 +7557,20 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>AplPay SPOTHERO 844-CHICAGO             IL</t>
+          <t>Subway 25044 7344857827 MI null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D223" t="n">
-        <v>15.83</v>
+        <v>12.6</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>Parking</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F223" t="n">
@@ -7589,20 +7589,20 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>COMPASSIONATE CARE AANN ARBOR           MI</t>
+          <t>AplPay SPOTHERO 844-CHICAGO             IL</t>
         </is>
       </c>
       <c r="D224" t="n">
-        <v>248.12</v>
+        <v>15.83</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Medical</t>
+          <t>Parking</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -7621,20 +7621,20 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Subway 25044 7344857827 MI null XXXXXXXXXXXX9868</t>
+          <t>COMPASSIONATE CARE AANN ARBOR           MI</t>
         </is>
       </c>
       <c r="D225" t="n">
-        <v>12.6</v>
+        <v>248.12</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Medical</t>
         </is>
       </c>
       <c r="F225" t="n">
@@ -7653,20 +7653,20 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>AMEX RIDESHARE CREDIT</t>
+          <t>MENDOCINO FARMS #36 SAN FRANCISCO CA null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D226" t="n">
-        <v>-10</v>
+        <v>15.69</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F226" t="n">
@@ -7685,20 +7685,20 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>UBER</t>
+          <t>MJ SUSHI FREMONT CA</t>
         </is>
       </c>
       <c r="D227" t="n">
-        <v>61.91</v>
+        <v>50.69</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F227" t="n">
@@ -7717,20 +7717,20 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>MJ SUSHI FREMONT CA</t>
+          <t>AMEX RIDESHARE CREDIT</t>
         </is>
       </c>
       <c r="D228" t="n">
-        <v>50.69</v>
+        <v>-10</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F228" t="n">
@@ -7749,20 +7749,20 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>MENDOCINO FARMS #36 SAN FRANCISCO CA null XXXXXXXXXXXX9868</t>
+          <t>UBER</t>
         </is>
       </c>
       <c r="D229" t="n">
-        <v>15.69</v>
+        <v>61.91</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F229" t="n">
@@ -7877,20 +7877,20 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>HAIDILAO HOT POT FREMO FREMONT CA</t>
+          <t>AT&amp;T UVERSE PAYMENT 8002882020          TX</t>
         </is>
       </c>
       <c r="D233" t="n">
-        <v>100.56</v>
+        <v>55.22</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="F233" t="n">
@@ -7946,15 +7946,15 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>AT&amp;T UVERSE PAYMENT 8002882020          TX</t>
+          <t>AplPay TARGET       FREMONT             CA</t>
         </is>
       </c>
       <c r="D235" t="n">
-        <v>55.22</v>
+        <v>11.01</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F235" t="n">
@@ -7973,20 +7973,20 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>TST* BARNEYS GOURMET H Berkeley CA</t>
+          <t>UNITED PACIFIC #5734FREMONT             CA</t>
         </is>
       </c>
       <c r="D236" t="n">
-        <v>104.1</v>
+        <v>10</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F236" t="n">
@@ -8010,15 +8010,15 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>AplPay TARGET       FREMONT             CA</t>
+          <t>AplPay UNIQLO USA LLNEW YORK            NY</t>
         </is>
       </c>
       <c r="D237" t="n">
-        <v>11.01</v>
+        <v>16.3</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Shopping</t>
         </is>
       </c>
       <c r="F237" t="n">
@@ -8037,20 +8037,20 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>AplPay UNIQLO USA LLNEW YORK            NY</t>
+          <t>HAIDILAO HOT POT FREMO FREMONT CA</t>
         </is>
       </c>
       <c r="D238" t="n">
-        <v>16.3</v>
+        <v>100.56</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Shopping</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F238" t="n">
@@ -8069,20 +8069,20 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>UNITED PACIFIC #5734FREMONT             CA</t>
+          <t>TST* BARNEYS GOURMET H Berkeley CA</t>
         </is>
       </c>
       <c r="D239" t="n">
-        <v>10</v>
+        <v>104.1</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F239" t="n">
@@ -8170,11 +8170,11 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>TOUS LES JOURS FREMONT FREMONT CA null XXXXXXXXXXXX9868</t>
+          <t>TST* TAISHOKEN RAMEN San Mateo CA</t>
         </is>
       </c>
       <c r="D242" t="n">
-        <v>10.15</v>
+        <v>103.38</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -8202,11 +8202,11 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>TST* TAISHOKEN RAMEN San Mateo CA</t>
+          <t>TOUS LES JOURS FREMONT FREMONT CA null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D243" t="n">
-        <v>103.38</v>
+        <v>10.15</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -8522,15 +8522,15 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>CHIPOTLE ONLINE CHIPOTLE.COM CA</t>
+          <t>Costco Annual Membership Renewal 1-800-7</t>
         </is>
       </c>
       <c r="D253" t="n">
-        <v>13.83</v>
+        <v>120</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F253" t="n">
@@ -8554,15 +8554,15 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Costco Annual Membership Renewal 1-800-7</t>
+          <t>CHIPOTLE ONLINE CHIPOTLE.COM CA</t>
         </is>
       </c>
       <c r="D254" t="n">
-        <v>120</v>
+        <v>13.83</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F254" t="n">
@@ -8613,20 +8613,20 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>AplPay STARBUCKS    800-782-7282        WA</t>
+          <t>VENTRA ACCOUNT CHICAGO IL</t>
         </is>
       </c>
       <c r="D256" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F256" t="n">
@@ -8645,20 +8645,20 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Delta SkyMiles® Gold Card </t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>VENTRA ACCOUNT CHICAGO IL</t>
+          <t>AplPay STARBUCKS    800-782-7282        WA</t>
         </is>
       </c>
       <c r="D257" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F257" t="n">
@@ -8677,20 +8677,20 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>AplPay GEICO AUTO   (800)841-3000       DC</t>
+          <t>PY *KUNG FU TEA - HOLL HOLLAND MI null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D258" t="n">
-        <v>358.89</v>
+        <v>7</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Car Maintenance</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F258" t="n">
@@ -8709,20 +8709,20 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>PY *KUNG FU TEA - HOLL HOLLAND MI null XXXXXXXXXXXX9868</t>
+          <t>AplPay GEICO AUTO   (800)841-3000       DC</t>
         </is>
       </c>
       <c r="D259" t="n">
-        <v>7</v>
+        <v>358.89</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Car Maintenance</t>
         </is>
       </c>
       <c r="F259" t="n">
@@ -8874,15 +8874,15 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>RUTH'S CHRIS STEAK HOUSE ANN ARBOR MI</t>
+          <t>MARIANOS #503 CHICAGO IL</t>
         </is>
       </c>
       <c r="D264" t="n">
-        <v>70</v>
+        <v>15.82</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -8906,15 +8906,15 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>MARIANOS #503 CHICAGO IL</t>
+          <t>RUTH'S CHRIS STEAK HOUSE ANN ARBOR MI</t>
         </is>
       </c>
       <c r="D265" t="n">
-        <v>15.82</v>
+        <v>70</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F265" t="n">
@@ -9061,20 +9061,20 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #0744 WYOMING MI</t>
+          <t>AplPay TRADER JOE S KENTWOOD            MI</t>
         </is>
       </c>
       <c r="D270" t="n">
-        <v>55.09</v>
+        <v>44.88</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F270" t="n">
@@ -9093,16 +9093,16 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>AplPay TRADER JOE S KENTWOOD            MI</t>
+          <t>MARIANOS #503 CHICAGO IL</t>
         </is>
       </c>
       <c r="D271" t="n">
-        <v>44.88</v>
+        <v>11.23</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -9125,20 +9125,20 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>AplPay WHOLEFDS GRP GRAND RAPIDS        MI</t>
+          <t>COSTCO WHSE #0744 WYOMING MI</t>
         </is>
       </c>
       <c r="D272" t="n">
-        <v>34.26</v>
+        <v>55.09</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F272" t="n">
@@ -9157,16 +9157,16 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>MARIANOS #503 CHICAGO IL</t>
+          <t>AplPay WHOLEFDS GRP GRAND RAPIDS        MI</t>
         </is>
       </c>
       <c r="D273" t="n">
-        <v>11.23</v>
+        <v>34.26</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -9189,20 +9189,20 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>VENTRA ACCOUNT CHICAGO IL</t>
+          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
         </is>
       </c>
       <c r="D274" t="n">
-        <v>2.25</v>
+        <v>6.79</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F274" t="n">
@@ -9226,15 +9226,15 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>MARIANOS #503 CHICAGO IL</t>
+          <t>VENTRA ACCOUNT CHICAGO IL</t>
         </is>
       </c>
       <c r="D275" t="n">
-        <v>10.21</v>
+        <v>2.25</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F275" t="n">
@@ -9253,16 +9253,16 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
+          <t>MARIANOS #503 CHICAGO IL</t>
         </is>
       </c>
       <c r="D276" t="n">
-        <v>6.79</v>
+        <v>10.21</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -9413,20 +9413,20 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>OURHOME CATERING MICHIGANHOLLAND MI</t>
+          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
         </is>
       </c>
       <c r="D281" t="n">
-        <v>5.3</v>
+        <v>3.69</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F281" t="n">
@@ -9445,20 +9445,20 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
+          <t>OURHOME CATERING MICHIGANHOLLAND MI</t>
         </is>
       </c>
       <c r="D282" t="n">
-        <v>3.69</v>
+        <v>5.3</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F282" t="n">
@@ -9514,15 +9514,15 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>GREYHOUND Los Angeles CA</t>
+          <t>GINZA SUSHI &amp; RAMEN. GRAND RAPIDS MI</t>
         </is>
       </c>
       <c r="D284" t="n">
-        <v>32.98</v>
+        <v>41</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F284" t="n">
@@ -9546,15 +9546,15 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>GINZA SUSHI &amp; RAMEN. GRAND RAPIDS MI</t>
+          <t>GREYHOUND Los Angeles CA</t>
         </is>
       </c>
       <c r="D285" t="n">
-        <v>41</v>
+        <v>32.98</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F285" t="n">
@@ -9637,20 +9637,20 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>OURHOME CATERING MICHI HOLLAND MI null XXXXXXXXXXXX9868</t>
+          <t>MARIANOS #503 CHICAGO IL</t>
         </is>
       </c>
       <c r="D288" t="n">
-        <v>5.3</v>
+        <v>21.34</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F288" t="n">
@@ -9701,20 +9701,20 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>MARIANOS #503 CHICAGO IL</t>
+          <t>OURHOME CATERING MICHI HOLLAND MI null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D290" t="n">
-        <v>21.34</v>
+        <v>5.3</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F290" t="n">
@@ -9898,15 +9898,15 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>OURHOME CATERING MICHIGANHOLLAND MI</t>
+          <t>DELTA AIR 0067114765845SEATTLE WANAME: KUO/YUEHLUNG DEPART:08/28/2024 LAX TO SFO: DL: CLASS:E : STOP: O  TO : : CLASS: : STOP: O</t>
         </is>
       </c>
       <c r="D296" t="n">
-        <v>5.3</v>
+        <v>48.48</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F296" t="n">
@@ -9930,11 +9930,11 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>EXPEDIA 72883483935892 EXPEDIA.COM WA</t>
+          <t>UNITED 0162407842682UNITED.COM TXNAME: KUO/YUEHLUNG DEPART:08/13/2024 SFO TO TPE: UA: CLASS:Y : STOP: X  TO SFO: UA: CLASS:Y : STOP: O</t>
         </is>
       </c>
       <c r="D297" t="n">
-        <v>1.42</v>
+        <v>38.6</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -9962,11 +9962,11 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>ALASKA AIR 0277114769813SEATTLE WANAME: KUO/YUEHLUNG DEPART:08/23/2024 SFO TO LAX: AS: CLASS:O : STOP: O</t>
+          <t>EXPEDIA 72883483935892 EXPEDIA.COM WA</t>
         </is>
       </c>
       <c r="D298" t="n">
-        <v>58.1</v>
+        <v>1.42</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -9994,15 +9994,15 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>DELTA AIR 0067114765845SEATTLE WANAME: KUO/YUEHLUNG DEPART:08/28/2024 LAX TO SFO: DL: CLASS:E : STOP: O  TO : : CLASS: : STOP: O</t>
+          <t>OURHOME CATERING MICHIGANHOLLAND MI</t>
         </is>
       </c>
       <c r="D299" t="n">
-        <v>48.48</v>
+        <v>5.3</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F299" t="n">
@@ -10026,11 +10026,11 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>UNITED 0162407842682UNITED.COM TXNAME: KUO/YUEHLUNG DEPART:08/13/2024 SFO TO TPE: UA: CLASS:Y : STOP: X  TO SFO: UA: CLASS:Y : STOP: O</t>
+          <t>ALASKA AIR 0277114769813SEATTLE WANAME: KUO/YUEHLUNG DEPART:08/23/2024 SFO TO LAX: AS: CLASS:O : STOP: O</t>
         </is>
       </c>
       <c r="D300" t="n">
-        <v>38.6</v>
+        <v>58.1</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -10218,15 +10218,15 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>UNITED 0164421641210UNITED.COM TXNAME:  DEPART:</t>
+          <t>TST* MIZU SUSHI Holland MI</t>
         </is>
       </c>
       <c r="D306" t="n">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F306" t="n">
@@ -10250,15 +10250,15 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>TST* MIZU SUSHI Holland MI</t>
+          <t>UNITED 0164421641210UNITED.COM TXNAME:  DEPART:</t>
         </is>
       </c>
       <c r="D307" t="n">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F307" t="n">
@@ -10277,20 +10277,20 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
+          <t>UA INFLT 0164421641259HOUSTON TXNAME:  DEPART:</t>
         </is>
       </c>
       <c r="D308" t="n">
-        <v>12.54</v>
+        <v>8</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F308" t="n">
@@ -10309,20 +10309,20 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>UA INFLT 0164421641259HOUSTON TXNAME:  DEPART:</t>
+          <t>AplPay MEIJER # 047 HOLLAND             MI</t>
         </is>
       </c>
       <c r="D309" t="n">
-        <v>8</v>
+        <v>12.54</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F309" t="n">
@@ -10446,7 +10446,7 @@
         </is>
       </c>
       <c r="D313" t="n">
-        <v>5.3</v>
+        <v>1.33</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -10478,7 +10478,7 @@
         </is>
       </c>
       <c r="D314" t="n">
-        <v>1.33</v>
+        <v>5.3</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -10602,11 +10602,11 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>UNITED 0164423008225UNITED.COM TXNAME:  DEPART:</t>
+          <t>UNITED 0164423008224UNITED.COM TXNAME:  DEPART:</t>
         </is>
       </c>
       <c r="D318" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -10634,11 +10634,11 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>UNITED 0164423008224UNITED.COM TXNAME:  DEPART:</t>
+          <t>UNITED 0164423008225UNITED.COM TXNAME:  DEPART:</t>
         </is>
       </c>
       <c r="D319" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -10885,20 +10885,20 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>APPLE.COM/BILL      INTERNET CHARGE     CA</t>
+          <t>CHIPOTLE 1846 MUNSTER IN</t>
         </is>
       </c>
       <c r="D327" t="n">
-        <v>9.99</v>
+        <v>24.82</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Subscriptions</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F327" t="n">
@@ -10954,15 +10954,15 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>CHIPOTLE 1846 MUNSTER IN</t>
+          <t>TESLA SUPERCHARGER US 877-7983752 CA</t>
         </is>
       </c>
       <c r="D329" t="n">
-        <v>24.82</v>
+        <v>12.24</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F329" t="n">
@@ -10986,15 +10986,15 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>TESLA SUPERCHARGER US 877-7983752 CA</t>
+          <t>COSTCO WHSE #1107 CHICAGO IL</t>
         </is>
       </c>
       <c r="D330" t="n">
-        <v>12.24</v>
+        <v>45.66</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F330" t="n">
@@ -11013,20 +11013,20 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #1107 CHICAGO IL</t>
+          <t>APPLE.COM/BILL      INTERNET CHARGE     CA</t>
         </is>
       </c>
       <c r="D331" t="n">
-        <v>45.66</v>
+        <v>9.99</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Subscriptions</t>
         </is>
       </c>
       <c r="F331" t="n">
@@ -11050,11 +11050,11 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>NOODLES ETC CHICAGO IL null XXXXXXXXXXXX9868</t>
+          <t>5GUYS 4020 QSR CHICAGO IL null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D332" t="n">
-        <v>27.92</v>
+        <v>18.75</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -11077,20 +11077,20 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>AplPay VENTRA ACCOUNCHICAGO             IL</t>
+          <t>NOODLES ETC CHICAGO IL null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D333" t="n">
-        <v>2.25</v>
+        <v>27.92</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F333" t="n">
@@ -11109,20 +11109,20 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>5GUYS 4020 QSR CHICAGO IL null XXXXXXXXXXXX9868</t>
+          <t>AplPay VENTRA ACCOUNCHICAGO             IL</t>
         </is>
       </c>
       <c r="D334" t="n">
-        <v>18.75</v>
+        <v>2.25</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F334" t="n">
@@ -11274,15 +11274,15 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>AMEX RIDESHARE CREDIT</t>
+          <t>AplPay TARGET       FREMONT             CA</t>
         </is>
       </c>
       <c r="D339" t="n">
-        <v>-10</v>
+        <v>22.04</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F339" t="n">
@@ -11301,20 +11301,20 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>AplPay LYFT         855-280-0278        CA</t>
+          <t>COSTCO WHSE #0778 FREMONT CA</t>
         </is>
       </c>
       <c r="D340" t="n">
-        <v>47.99</v>
+        <v>232.5</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Rideshare</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F340" t="n">
@@ -11333,20 +11333,20 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>AplPay TARGET       FREMONT             CA</t>
+          <t>EXPEDIA 72895132839660 EXPEDIA.COM WA</t>
         </is>
       </c>
       <c r="D341" t="n">
-        <v>22.04</v>
+        <v>11.54</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F341" t="n">
@@ -11365,20 +11365,20 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>EXPEDIA 72895132839660 EXPEDIA.COM WA</t>
+          <t>SQ *RAMEN NAGI VALLEY Santa Clara CA null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D342" t="n">
-        <v>11.54</v>
+        <v>46.61</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F342" t="n">
@@ -11397,20 +11397,20 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #0778 FREMONT CA</t>
+          <t>SQ *LUCKY TEA VALLEY F Santa Clara CA null XXXXXXXXXXXX9868</t>
         </is>
       </c>
       <c r="D343" t="n">
-        <v>232.5</v>
+        <v>5.48</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F343" t="n">
@@ -11429,20 +11429,20 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Blue Cash Preferred® </t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>SQ *LUCKY TEA VALLEY F Santa Clara CA null XXXXXXXXXXXX9868</t>
+          <t>AplPay MARIANOS #503CHICAGO             IL</t>
         </is>
       </c>
       <c r="D344" t="n">
-        <v>5.48</v>
+        <v>10.1</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Groceries</t>
         </is>
       </c>
       <c r="F344" t="n">
@@ -11461,20 +11461,20 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>SQ *RAMEN NAGI VALLEY Santa Clara CA null XXXXXXXXXXXX9868</t>
+          <t>AMEX RIDESHARE CREDIT</t>
         </is>
       </c>
       <c r="D345" t="n">
-        <v>46.61</v>
+        <v>-10</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F345" t="n">
@@ -11493,20 +11493,20 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t xml:space="preserve">Blue Cash Preferred® </t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>AplPay MARIANOS #503CHICAGO             IL</t>
+          <t>AplPay LYFT         855-280-0278        CA</t>
         </is>
       </c>
       <c r="D346" t="n">
-        <v>10.1</v>
+        <v>47.99</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Groceries</t>
+          <t>Rideshare</t>
         </is>
       </c>
       <c r="F346" t="n">
@@ -11525,20 +11525,20 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>Costco</t>
+          <t>Custom Cash</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>COSTCO WHSE #0778 FREMONT CA</t>
+          <t>MJ SUSHI FREMONT CA</t>
         </is>
       </c>
       <c r="D347" t="n">
-        <v>63.03</v>
+        <v>78.84</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Merchandise and Wholesale</t>
+          <t>Dining</t>
         </is>
       </c>
       <c r="F347" t="n">
@@ -11557,16 +11557,16 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
+          <t>Costco</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>WAL-MART 2989 2989  FREMONT             CA</t>
+          <t>COSTCO WHSE #0778 FREMONT CA</t>
         </is>
       </c>
       <c r="D348" t="n">
-        <v>17.07</v>
+        <v>63.03</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -11621,20 +11621,20 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>Custom Cash</t>
+          <t xml:space="preserve">Delta SkyMiles® Platinum Card </t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>MJ SUSHI FREMONT CA</t>
+          <t>WAL-MART 2989 2989  FREMONT             CA</t>
         </is>
       </c>
       <c r="D350" t="n">
-        <v>78.84</v>
+        <v>17.07</v>
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Dining</t>
+          <t>Merchandise and Wholesale</t>
         </is>
       </c>
       <c r="F350" t="n">
@@ -11754,15 +11754,15 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>COSTCO GAS #0569 COMMERCE CA</t>
+          <t>EXPEDIA 72895132839660 EXPEDIA.COM WA</t>
         </is>
       </c>
       <c r="D354" t="n">
-        <v>46.83</v>
+        <v>-11.54</v>
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>Charging and Gas</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="F354" t="n">
@@ -11786,15 +11786,15 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>EXPEDIA 72895132839660 EXPEDIA.COM WA</t>
+          <t>COSTCO GAS #0569 COMMERCE CA</t>
         </is>
       </c>
       <c r="D355" t="n">
-        <v>-11.54</v>
+        <v>46.83</v>
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Charging and Gas</t>
         </is>
       </c>
       <c r="F355" t="n">

</xml_diff>